<commit_message>
spelling changes in data
</commit_message>
<xml_diff>
--- a/data/Sub_littoral_mud.xlsx
+++ b/data/Sub_littoral_mud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\working\Development\R\meso-tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705BDC91-1201-487B-B090-A393FFE23B8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B26013-2E95-42E7-B044-875169074B2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28020" windowHeight="14355" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="109">
   <si>
     <t>Time</t>
   </si>
@@ -353,6 +353,9 @@
   </si>
   <si>
     <t>Burrow holothurians</t>
+  </si>
+  <si>
+    <t>Echinoids</t>
   </si>
 </sst>
 </file>
@@ -2244,10 +2247,10 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2303,7 +2306,7 @@
         <v>106</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="O1" s="17" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
git revert borked mud spreadsheet
</commit_message>
<xml_diff>
--- a/data/Sub_littoral_mud.xlsx
+++ b/data/Sub_littoral_mud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\working\Development\R\meso-tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B26013-2E95-42E7-B044-875169074B2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705BDC91-1201-487B-B090-A393FFE23B8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28020" windowHeight="14355" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="108">
   <si>
     <t>Time</t>
   </si>
@@ -353,9 +353,6 @@
   </si>
   <si>
     <t>Burrow holothurians</t>
-  </si>
-  <si>
-    <t>Echinoids</t>
   </si>
 </sst>
 </file>
@@ -2247,10 +2244,10 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M28" sqref="M28"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2306,7 +2303,7 @@
         <v>106</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="O1" s="17" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
spelling fixes in data
</commit_message>
<xml_diff>
--- a/data/Sub_littoral_mud.xlsx
+++ b/data/Sub_littoral_mud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\working\Development\R\meso-tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705BDC91-1201-487B-B090-A393FFE23B8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB265140-CD1C-4F80-8AF9-EAEDC606D592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28020" windowHeight="14355" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,9 +103,6 @@
     <t>Mobile epi pred scav</t>
   </si>
   <si>
-    <t>Echin</t>
-  </si>
-  <si>
     <t>Attachd epi</t>
   </si>
   <si>
@@ -353,6 +350,9 @@
   </si>
   <si>
     <t>Burrow holothurians</t>
+  </si>
+  <si>
+    <t>Echinoids</t>
   </si>
 </sst>
 </file>
@@ -2244,10 +2244,10 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2279,7 +2279,7 @@
         <v>18</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>19</v>
@@ -2297,16 +2297,16 @@
         <v>23</v>
       </c>
       <c r="L1" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="17" t="s">
-        <v>106</v>
-      </c>
       <c r="N1" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" s="17" t="s">
         <v>24</v>
-      </c>
-      <c r="O1" s="17" t="s">
-        <v>25</v>
       </c>
       <c r="P1" s="18"/>
       <c r="Q1" s="18"/>
@@ -2318,236 +2318,236 @@
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="F2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="21" t="s">
+      <c r="I2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="J2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="21" t="s">
+      <c r="L2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="21" t="s">
-        <v>31</v>
-      </c>
       <c r="M2" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>34</v>
-      </c>
       <c r="E3" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M3" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N3" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O3" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P3" s="24"/>
       <c r="Q3" s="24"/>
     </row>
     <row r="4" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="G4" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="H4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="K4" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="M4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="23" t="s">
         <v>36</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="M4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="O4" s="23" t="s">
-        <v>37</v>
       </c>
       <c r="P4" s="24"/>
       <c r="Q4" s="24"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M5" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N5" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O5" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P5" s="24"/>
       <c r="Q5" s="24"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K6" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L6" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M6" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N6" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O6" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P6" s="24"/>
       <c r="Q6" s="24"/>
@@ -2555,49 +2555,49 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>38</v>
-      </c>
       <c r="F7" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N7" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O7" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P7" s="24"/>
       <c r="Q7" s="24"/>
@@ -2605,301 +2605,301 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K8" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M8" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N8" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O8" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P8" s="24"/>
       <c r="Q8" s="24"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M9" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N9" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O9" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P9" s="24"/>
       <c r="Q9" s="24"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K10" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L10" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M10" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N10" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O10" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P10" s="24"/>
       <c r="Q10" s="24"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K11" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P11" s="24"/>
       <c r="Q11" s="24"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I12" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L12" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="26" t="s">
-        <v>38</v>
-      </c>
       <c r="N12" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P12" s="24"/>
       <c r="Q12" s="24"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>38</v>
-      </c>
       <c r="I13" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K13" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="L13" s="23" t="s">
-        <v>37</v>
-      </c>
       <c r="M13" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N13" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" s="23" t="s">
         <v>36</v>
-      </c>
-      <c r="O13" s="23" t="s">
-        <v>37</v>
       </c>
       <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="29"/>
       <c r="C14" s="18"/>
@@ -2920,7 +2920,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P15" s="32"/>
       <c r="Q15" s="32"/>
@@ -2946,7 +2946,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="18" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -2984,7 +2984,7 @@
     </row>
     <row r="19" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -3054,7 +3054,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
@@ -3073,13 +3073,13 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -3096,13 +3096,13 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
@@ -3119,7 +3119,7 @@
     </row>
     <row r="26" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
@@ -3556,95 +3556,95 @@
         <v>16</v>
       </c>
       <c r="D1" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="F1" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="G1" s="36" t="s">
         <v>62</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
       <c r="D2" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="40" t="s">
-        <v>67</v>
-      </c>
       <c r="F3" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="40" t="s">
         <v>66</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G4" s="42"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="42" t="s">
         <v>69</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>70</v>
       </c>
       <c r="E5" s="42"/>
       <c r="F5" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5" s="42"/>
     </row>
@@ -3654,162 +3654,162 @@
         <v>19</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="42"/>
       <c r="F6" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" s="42"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="42"/>
       <c r="F7" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G7" s="42"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G8" s="42"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E9" s="42"/>
       <c r="F9" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G9" s="42"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" s="42"/>
       <c r="F10" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G10" s="42"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="21"/>
       <c r="B11" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G11" s="42"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="21"/>
       <c r="B12" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="42"/>
       <c r="E12" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G12" s="42"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="21"/>
       <c r="B13" s="17" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="42"/>
       <c r="F13" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G13" s="42"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="21"/>
       <c r="B14" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="42"/>
       <c r="E14" s="42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F14" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G14" s="42"/>
     </row>
@@ -3842,7 +3842,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
@@ -3870,7 +3870,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
@@ -3880,13 +3880,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
@@ -3895,13 +3895,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
@@ -3914,7 +3914,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -3927,7 +3927,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
@@ -3935,13 +3935,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
@@ -3949,13 +3949,13 @@
     </row>
     <row r="27" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="28" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
@@ -4100,65 +4100,65 @@
         <v>16</v>
       </c>
       <c r="D1" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="F1" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="G1" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="H1" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="I1" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="J1" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="K1" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="L1" s="50" t="s">
         <v>84</v>
-      </c>
-      <c r="L1" s="50" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
       <c r="D2" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="H2" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="I2" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="J2" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" s="52" t="s">
         <v>87</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="K2" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="L2" s="52" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -4167,36 +4167,36 @@
         <v>1</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="51"/>
       <c r="F3" s="51"/>
       <c r="G3" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3" s="51"/>
       <c r="I3" s="51"/>
       <c r="J3" s="51"/>
       <c r="K3" s="51"/>
       <c r="L3" s="53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
       <c r="G4" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H4" s="22"/>
       <c r="I4" s="21"/>
@@ -4206,25 +4206,25 @@
     </row>
     <row r="5" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="54" t="s">
         <v>89</v>
-      </c>
-      <c r="E5" s="54" t="s">
-        <v>90</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="22"/>
       <c r="I5" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J5" s="21"/>
       <c r="K5" s="21"/>
@@ -4232,23 +4232,23 @@
     </row>
     <row r="6" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
       <c r="I6" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J6" s="21"/>
       <c r="K6" s="21"/>
@@ -4257,17 +4257,17 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
       <c r="B7" s="36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F7" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
@@ -4278,13 +4278,13 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="B8" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
@@ -4292,7 +4292,7 @@
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L8" s="24"/>
     </row>
@@ -4302,7 +4302,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
@@ -4311,7 +4311,7 @@
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
       <c r="K9" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L9" s="24"/>
     </row>
@@ -4321,7 +4321,7 @@
         <v>21</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="21"/>
@@ -4330,7 +4330,7 @@
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L10" s="24"/>
     </row>
@@ -4340,7 +4340,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
@@ -4349,17 +4349,17 @@
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
       <c r="K11" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L11" s="24"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="21"/>
       <c r="B12" s="17" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
@@ -4368,7 +4368,7 @@
       <c r="I12" s="21"/>
       <c r="J12" s="21"/>
       <c r="K12" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L12" s="24"/>
     </row>
@@ -4388,7 +4388,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="45"/>
       <c r="C14" s="45"/>
@@ -4402,19 +4402,19 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
       <c r="H15" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I15" s="21"/>
       <c r="J15" s="21"/>
@@ -4423,39 +4423,39 @@
     </row>
     <row r="16" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
       <c r="G16" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16" s="21"/>
       <c r="I16" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
@@ -4486,7 +4486,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
@@ -4502,7 +4502,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -4518,7 +4518,7 @@
     </row>
     <row r="22" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -4650,32 +4650,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
@@ -4685,32 +4685,32 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="58" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>